<commit_message>
Updated the existing project
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Browsers" sheetId="14" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="211">
   <si>
     <t>Runmode</t>
   </si>
@@ -169,9 +169,6 @@
     <t>verifyingPhysicianGrid</t>
   </si>
   <si>
-    <t>Physicians</t>
-  </si>
-  <si>
     <t>PHYSICIANS</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>PhoneNumber</t>
   </si>
   <si>
-    <t>(123) 456-789</t>
-  </si>
-  <si>
     <t>saveHospiceElection</t>
   </si>
   <si>
@@ -250,9 +244,6 @@
     <t>addInsuranceCarrier</t>
   </si>
   <si>
-    <t>InsuranceCarrier</t>
-  </si>
-  <si>
     <t>InsuranceAddress</t>
   </si>
   <si>
@@ -271,12 +262,6 @@
     <t>insuranceCarrierUpdate</t>
   </si>
   <si>
-    <t>PhoneType</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
     <t>addMedicareIntermediary</t>
   </si>
   <si>
@@ -316,12 +301,6 @@
     <t>updatePhysicianServicesRecord</t>
   </si>
   <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>tier</t>
-  </si>
-  <si>
     <t>GroupName</t>
   </si>
   <si>
@@ -376,9 +355,6 @@
     <t>LanguageName</t>
   </si>
   <si>
-    <t>Arabic</t>
-  </si>
-  <si>
     <t>fromDate_Month</t>
   </si>
   <si>
@@ -545,9 +521,6 @@
   </si>
   <si>
     <t>AssingedOffices</t>
-  </si>
-  <si>
-    <t>What about other fields?</t>
   </si>
   <si>
     <t>We don't need this data</t>
@@ -633,12 +606,82 @@
   <si>
     <t>Palliative Care</t>
   </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Payer Type</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>mumms</t>
+  </si>
+  <si>
+    <t>MaxDaysCoverage</t>
+  </si>
+  <si>
+    <t>RepeatLastPeriod</t>
+  </si>
+  <si>
+    <t>F2FVisitsRequiredStartingonElectionPeriod</t>
+  </si>
+  <si>
+    <t>ReadmissiontoHospiceAllowed</t>
+  </si>
+  <si>
+    <t>StartElectionOneOnReadmission</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+ElectionsRequired</t>
+  </si>
+  <si>
+    <t>Auto-Certified</t>
+  </si>
+  <si>
+    <t>(866) 466-1234</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ThisIsADummyLanguageNameToTestTheUIOfTheApplication</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>NPI</t>
+  </si>
+  <si>
+    <t>HeaderText</t>
+  </si>
+  <si>
+    <t>Acker</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Rutherfordton</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +721,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -820,7 +868,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -858,7 +906,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
@@ -888,6 +935,12 @@
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -1227,7 +1280,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1235,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1248,7 +1301,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,14 +1497,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>11</v>
+      <c r="A2" s="32" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
@@ -1460,7 +1513,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" s="12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>2</v>
@@ -1615,8 +1668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A124" sqref="A1:A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,9 +1677,9 @@
     <col min="1" max="1" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -1657,54 +1710,54 @@
       <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>179</v>
+      <c r="G2" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="26">
+      <c r="A3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="25">
         <v>571</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>177</v>
+      <c r="C4" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1722,10 +1775,10 @@
       <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1733,24 +1786,24 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="26">
+      <c r="A7" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="25">
         <v>571</v>
       </c>
-      <c r="E7" s="26"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1770,22 +1823,22 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>128</v>
+      <c r="A11" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1803,22 +1856,22 @@
       <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>103</v>
+      <c r="D14" s="24" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>104</v>
+      <c r="A15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1838,12 +1891,12 @@
       <c r="A19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>183</v>
+      <c r="B19" s="22" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1859,12 +1912,12 @@
       <c r="A23" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>134</v>
+      <c r="B23" s="22" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1872,13 +1925,13 @@
       <c r="A26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="24" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1886,18 +1939,18 @@
       <c r="A27" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27" s="23">
+      <c r="B27" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="22">
         <v>253</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>136</v>
+      <c r="D27" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1905,16 +1958,16 @@
       <c r="A30" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="24" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1922,25 +1975,25 @@
       <c r="A31" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E31" s="23">
+      <c r="B31" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="22">
         <v>253</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>1</v>
       </c>
@@ -1951,126 +2004,167 @@
         <v>47</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="23" t="s">
-        <v>138</v>
+      <c r="B35" s="22" t="s">
+        <v>130</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="25"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" s="24"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="36">
+        <v>1750474573</v>
+      </c>
+      <c r="G43" s="2">
+        <v>70130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="2" t="s">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D50" s="24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>2</v>
       </c>
@@ -2078,32 +2172,32 @@
         <v>48</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D51" s="24" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="D54" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>2</v>
       </c>
@@ -2111,312 +2205,509 @@
         <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="F59" s="2">
+        <v>28139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F63" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="E70" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I70" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="C71" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="D71" s="23">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="E71" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F71" s="2">
+        <v>3</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I74" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" s="23">
+        <v>60</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F75" s="2">
+        <v>3</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E78" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F78" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H78" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="23" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D62" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="23" t="s">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="E79" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F79" s="2">
+        <v>70130</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="1"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E82" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F82" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E83" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F83" s="2">
+        <v>70130</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E86" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F86" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E87" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F87" s="2">
+        <v>70130</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D63" s="23" t="s">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D91" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="E63" s="23" t="s">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F63" s="23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="C67" s="23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" s="2" t="s">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" s="23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B78" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F78" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="G78" s="23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C79" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="D79" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D91" s="24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -2424,16 +2715,16 @@
         <v>1</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -2441,21 +2732,21 @@
         <v>2</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D99" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E99" s="24" t="s">
-        <v>152</v>
+        <v>82</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -2463,25 +2754,25 @@
         <v>1</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D102" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E102" s="24" t="s">
-        <v>160</v>
+        <v>88</v>
+      </c>
+      <c r="D102" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E102" s="23" t="s">
+        <v>152</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -2489,30 +2780,30 @@
         <v>2</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D103" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E103" s="24" t="s">
-        <v>128</v>
+        <v>91</v>
+      </c>
+      <c r="D103" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E103" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G103" s="28" t="s">
-        <v>159</v>
+        <v>149</v>
+      </c>
+      <c r="G103" s="27" t="s">
+        <v>151</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -2520,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -2528,29 +2819,29 @@
         <v>2</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B110" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C110" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D110" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="E110" s="23" t="s">
-        <v>167</v>
+      <c r="B110" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C110" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D110" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E110" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -2558,15 +2849,21 @@
         <v>2</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
+      </c>
+      <c r="D111" s="23">
+        <v>100</v>
+      </c>
+      <c r="E111" s="34">
+        <v>42438</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -2581,7 +2878,7 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -2589,56 +2886,56 @@
         <v>1</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D117" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="E117" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D117" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E117" s="23" t="s">
         <v>34</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B118" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C118" s="2">
-        <v>11</v>
-      </c>
-      <c r="D118" s="24">
+      <c r="B118" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C118" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D118" s="23">
         <v>2014</v>
       </c>
-      <c r="E118" s="24" t="s">
-        <v>115</v>
+      <c r="E118" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H118" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A119" s="20" t="s">
-        <v>117</v>
+      <c r="A119" s="19" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -2646,7 +2943,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -2654,15 +2951,15 @@
         <v>2</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D121" s="24" t="s">
-        <v>189</v>
+        <v>201</v>
+      </c>
+      <c r="D121" s="23" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A122" s="20" t="s">
-        <v>184</v>
+      <c r="A122" s="19" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -2670,56 +2967,56 @@
         <v>1</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J123" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M123" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="K123" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="L123" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="M123" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B124" s="21">
+      <c r="B124" s="20">
         <v>1</v>
       </c>
       <c r="C124" s="2">
         <v>10</v>
       </c>
-      <c r="D124" s="24">
+      <c r="D124" s="23">
         <v>2016</v>
       </c>
-      <c r="E124" s="24">
+      <c r="E124" s="23">
         <v>2</v>
       </c>
       <c r="F124" s="2">
@@ -2729,22 +3026,22 @@
         <v>2016</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="M124" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compiled yet again and testing whether the changes are pulled or not
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1280,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1301,7 +1301,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1466,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Made changes to run the scripts in the docker using the selenium server
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="3150" tabRatio="768"/>
   </bookViews>
   <sheets>
     <sheet name="Browsers" sheetId="14" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="allTests" sheetId="8" r:id="rId3"/>
     <sheet name="Admin" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1280,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Added firefox capabilities to the script
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="3150" tabRatio="768"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="3150" tabRatio="768" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Browsers" sheetId="14" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Admin" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:D8"/>
 </workbook>
 </file>
 
@@ -1250,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1281,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1289,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1498,7 +1499,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>23</v>
@@ -1666,7 +1667,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M124"/>
+  <dimension ref="A1:R124"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A124" sqref="A1:A124"/>

</xml_diff>

<commit_message>
Merged all the changes to the git now. The build looks good.
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -750,13 +750,13 @@
     <t>HIS Report For Admission</t>
   </si>
   <si>
-    <t>testAddWidgets</t>
-  </si>
-  <si>
     <t>com.Mumms.scripts.Admin</t>
   </si>
   <si>
-    <t>testAddWidgetsName</t>
+    <t>testaddWidgetPatientByFacilityType</t>
+  </si>
+  <si>
+    <t>testaddWidgetPatientByPayerType</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1677,7 @@
         <v>233</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
@@ -1686,7 +1686,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>2</v>
@@ -1804,7 +1804,7 @@
   <dimension ref="A1:L159"/>
   <sheetViews>
     <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,7 +3698,7 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All set for the demo. Made changes to the ActionEngine.java, and Test Data
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Browsers" sheetId="14" r:id="rId1"/>
@@ -735,9 +735,6 @@
     <t>Annie</t>
   </si>
   <si>
-    <t>Crain</t>
-  </si>
-  <si>
     <t xml:space="preserve">AdminUser </t>
   </si>
   <si>
@@ -757,6 +754,9 @@
   </si>
   <si>
     <t>testaddWidgetPatientByPayerType</t>
+  </si>
+  <si>
+    <t>Daniel</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1599,10 +1599,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>231</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>232</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
@@ -1644,7 +1644,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>225</v>
@@ -1674,10 +1674,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
@@ -1686,7 +1686,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>2</v>
@@ -1697,7 +1697,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>2</v>
@@ -3544,7 +3544,7 @@
         <v>169</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
@@ -3698,7 +3698,7 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
@@ -3733,7 +3733,7 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
@@ -3773,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +3917,7 @@
         <v>229</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>

</xml_diff>

<commit_message>
Changed the test data to run in Chrome
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Browsers" sheetId="14" r:id="rId1"/>
@@ -810,7 +810,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -915,12 +915,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="60"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="34"/>
       </patternFill>
@@ -956,7 +950,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1019,23 +1013,19 @@
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="18" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="19" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="18" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="19" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="18" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -1349,7 +1339,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,7 +1368,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1386,7 +1376,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1399,7 +1389,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,8 +1585,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>12</v>
+      <c r="A2" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>230</v>
@@ -1640,8 +1630,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>12</v>
+      <c r="A6" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>232</v>
@@ -1670,8 +1660,8 @@
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>12</v>
+      <c r="A9" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>232</v>
@@ -1850,7 +1840,7 @@
       <c r="E2" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="37"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
     </row>
@@ -2219,7 +2209,7 @@
       <c r="D43" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="F43" s="35">
+      <c r="F43" s="34">
         <v>1750474573</v>
       </c>
       <c r="G43" s="2">
@@ -2498,7 +2488,7 @@
       <c r="H70" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I70" s="33" t="s">
+      <c r="I70" s="32" t="s">
         <v>184</v>
       </c>
       <c r="J70" s="1" t="s">
@@ -2567,7 +2557,7 @@
       <c r="H74" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I74" s="33" t="s">
+      <c r="I74" s="32" t="s">
         <v>184</v>
       </c>
       <c r="J74" s="1" t="s">
@@ -2995,13 +2985,13 @@
       <c r="D111" s="23">
         <v>100</v>
       </c>
-      <c r="E111" s="36" t="s">
+      <c r="E111" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="F111" s="34" t="s">
+      <c r="F111" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="G111" s="34" t="s">
+      <c r="G111" s="33" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3046,21 +3036,21 @@
       <c r="D115" s="23">
         <v>100</v>
       </c>
-      <c r="E115" s="36" t="s">
+      <c r="E115" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="F115" s="34" t="s">
+      <c r="F115" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="G115" s="34" t="s">
+      <c r="G115" s="33" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
-      <c r="E116" s="36"/>
-      <c r="F116" s="34"/>
-      <c r="G116" s="34"/>
+      <c r="E116" s="35"/>
+      <c r="F116" s="33"/>
+      <c r="G116" s="33"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
@@ -3100,7 +3090,7 @@
       <c r="B119" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C119" s="34" t="s">
+      <c r="C119" s="33" t="s">
         <v>101</v>
       </c>
       <c r="D119" s="25" t="s">
@@ -3121,7 +3111,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B120" s="20"/>
-      <c r="C120" s="34"/>
+      <c r="C120" s="33"/>
       <c r="D120" s="25"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
@@ -3773,7 +3763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3847,67 +3837,67 @@
       <c r="C2" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="40"/>
-      <c r="AJ2" s="40"/>
-      <c r="AK2" s="40"/>
-      <c r="AL2" s="40"/>
-      <c r="AM2" s="40"/>
-      <c r="AN2" s="40"/>
-      <c r="AO2" s="40"/>
-      <c r="AP2" s="40"/>
-      <c r="AQ2" s="40"/>
-      <c r="AR2" s="40"/>
-      <c r="AS2" s="38"/>
-      <c r="AT2" s="38"/>
-      <c r="AU2" s="38"/>
-      <c r="AV2" s="38"/>
-      <c r="AW2" s="38"/>
-      <c r="AX2" s="38"/>
-      <c r="AY2" s="38"/>
-      <c r="AZ2" s="38"/>
-      <c r="BA2" s="38"/>
-      <c r="BB2" s="38"/>
-      <c r="BC2" s="38"/>
-      <c r="BD2" s="38"/>
-      <c r="BE2" s="38"/>
-      <c r="BF2" s="38"/>
-      <c r="BG2" s="38"/>
-      <c r="BH2" s="38"/>
-      <c r="BI2" s="38"/>
-      <c r="BJ2" s="38"/>
-      <c r="BK2" s="38"/>
-      <c r="BL2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
+      <c r="AN2" s="39"/>
+      <c r="AO2" s="39"/>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="39"/>
+      <c r="AR2" s="39"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="37"/>
+      <c r="BK2" s="37"/>
+      <c r="BL2" s="37"/>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -3919,67 +3909,67 @@
       <c r="C3" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="38"/>
-      <c r="AD3" s="38"/>
-      <c r="AE3" s="38"/>
-      <c r="AF3" s="38"/>
-      <c r="AG3" s="38"/>
-      <c r="AH3" s="38"/>
-      <c r="AI3" s="39"/>
-      <c r="AJ3" s="39"/>
-      <c r="AK3" s="38"/>
-      <c r="AL3" s="38"/>
-      <c r="AM3" s="38"/>
-      <c r="AN3" s="38"/>
-      <c r="AO3" s="38"/>
-      <c r="AP3" s="38"/>
-      <c r="AQ3" s="38"/>
-      <c r="AR3" s="38"/>
-      <c r="AS3" s="38"/>
-      <c r="AT3" s="38"/>
-      <c r="AU3" s="38"/>
-      <c r="AV3" s="38"/>
-      <c r="AW3" s="38"/>
-      <c r="AX3" s="38"/>
-      <c r="AY3" s="38"/>
-      <c r="AZ3" s="38"/>
-      <c r="BA3" s="38"/>
-      <c r="BB3" s="38"/>
-      <c r="BC3" s="38"/>
-      <c r="BD3" s="38"/>
-      <c r="BE3" s="38"/>
-      <c r="BF3" s="38"/>
-      <c r="BG3" s="38"/>
-      <c r="BH3" s="38"/>
-      <c r="BI3" s="38"/>
-      <c r="BJ3" s="38"/>
-      <c r="BK3" s="38"/>
-      <c r="BL3" s="38"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="38"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AO3" s="37"/>
+      <c r="AP3" s="37"/>
+      <c r="AQ3" s="37"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="37"/>
+      <c r="AT3" s="37"/>
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
+      <c r="AW3" s="37"/>
+      <c r="AX3" s="37"/>
+      <c r="AY3" s="37"/>
+      <c r="AZ3" s="37"/>
+      <c r="BA3" s="37"/>
+      <c r="BB3" s="37"/>
+      <c r="BC3" s="37"/>
+      <c r="BD3" s="37"/>
+      <c r="BE3" s="37"/>
+      <c r="BF3" s="37"/>
+      <c r="BG3" s="37"/>
+      <c r="BH3" s="37"/>
+      <c r="BI3" s="37"/>
+      <c r="BJ3" s="37"/>
+      <c r="BK3" s="37"/>
+      <c r="BL3" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fail case - Demo
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="239">
   <si>
     <t>Runmode</t>
   </si>
@@ -757,6 +757,9 @@
   </si>
   <si>
     <t>Daniel</t>
+  </si>
+  <si>
+    <t>DIR</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1342,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1371,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1379,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1392,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1557,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1589,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>230</v>
@@ -1615,7 +1618,7 @@
         <v>212</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1626,12 +1629,12 @@
         <v>202</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>232</v>
@@ -1641,7 +1644,7 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1649,7 +1652,7 @@
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,7 +1664,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>232</v>
@@ -1671,7 +1674,7 @@
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1679,7 +1682,7 @@
         <v>235</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1690,7 +1693,7 @@
         <v>236</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L159"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+    <sheetView topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,7 +3213,7 @@
         <v>169</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>171</v>
+        <v>238</v>
       </c>
       <c r="L127" s="2" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
Added reports scripts to the existing project
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1125" windowWidth="14805" windowHeight="6990" tabRatio="768" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7275" windowHeight="1080" tabRatio="768" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Browsers" sheetId="14" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="282">
   <si>
     <t>Runmode</t>
   </si>
@@ -498,9 +498,6 @@
   </si>
   <si>
     <t>ShortName</t>
-  </si>
-  <si>
-    <t>It's optional</t>
   </si>
   <si>
     <t>Assing thhis role to a auser and than delete?</t>
@@ -636,9 +633,6 @@
     <t>NC</t>
   </si>
   <si>
-    <t>ThisIsADummyReligionNameToTestTheUIOfTheApplication</t>
-  </si>
-  <si>
     <t>Church</t>
   </si>
   <si>
@@ -735,7 +729,7 @@
     <t>Annie</t>
   </si>
   <si>
-    <t xml:space="preserve">AdminUser </t>
+    <t>Crain</t>
   </si>
   <si>
     <t>com.Mumms.scripts.Reports</t>
@@ -747,19 +741,154 @@
     <t>HIS Report For Admission</t>
   </si>
   <si>
+    <t>testAddWidgets</t>
+  </si>
+  <si>
     <t>com.Mumms.scripts.Admin</t>
   </si>
   <si>
-    <t>testaddWidgetPatientByFacilityType</t>
-  </si>
-  <si>
-    <t>testaddWidgetPatientByPayerType</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>DIR</t>
+    <t>testAddWidgetsName</t>
+  </si>
+  <si>
+    <t>Social Worker - Social Worker</t>
+  </si>
+  <si>
+    <t>Employee-All</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Site-Office</t>
+  </si>
+  <si>
+    <t>RoleInReport</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>employees</t>
+  </si>
+  <si>
+    <t>SITE/OFFICE: Community Care Hospice</t>
+  </si>
+  <si>
+    <t>ReportTitle</t>
+  </si>
+  <si>
+    <t>Contact List</t>
+  </si>
+  <si>
+    <t>testGenerateContactsListReport</t>
+  </si>
+  <si>
+    <t>testGenerateBereavedPersonsReport</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>02/14/16 - 03/15/16</t>
+  </si>
+  <si>
+    <t>Bereaved Persons</t>
+  </si>
+  <si>
+    <t>SiteInReport</t>
+  </si>
+  <si>
+    <t>Community Care Hospice</t>
+  </si>
+  <si>
+    <t>Referrals by Referral Source</t>
+  </si>
+  <si>
+    <t>ReferrralSourceType</t>
+  </si>
+  <si>
+    <t>StatusAfterReferral</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>testGenerateReferralsbyReferralSourceReport</t>
+  </si>
+  <si>
+    <t>testGeneratePatientDaysbyLevelofCareReport</t>
+  </si>
+  <si>
+    <t>Patient Days by Level of Care</t>
+  </si>
+  <si>
+    <t>Hospice of Orlando</t>
+  </si>
+  <si>
+    <t>PatientStatusInReport</t>
+  </si>
+  <si>
+    <t>Admitted during Report Period</t>
+  </si>
+  <si>
+    <t>WarningDays</t>
+  </si>
+  <si>
+    <t>WarningType</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>F2F Past Due or Coming Due</t>
+  </si>
+  <si>
+    <t>Upcoming F2F and Certifications</t>
+  </si>
+  <si>
+    <t>WarningTypeInReport</t>
+  </si>
+  <si>
+    <t>Patients Requiring Face to Face within</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>testGenerateCreditClaimBalanceReport</t>
+  </si>
+  <si>
+    <t>Credit Claim Balance Report</t>
+  </si>
+  <si>
+    <t>ReportingDate</t>
+  </si>
+  <si>
+    <t>Christianity</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>02/18/16 - 03/17/16</t>
+  </si>
+  <si>
+    <t>AdminUser</t>
+  </si>
+  <si>
+    <t>HIS Report For Discharge</t>
+  </si>
+  <si>
+    <t>ADMITTED</t>
   </si>
 </sst>
 </file>
@@ -953,7 +1082,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1032,6 +1161,9 @@
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -1392,7 +1524,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,10 +1686,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,10 +1724,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>230</v>
+        <v>279</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
@@ -1604,10 +1736,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" s="12" t="s">
-        <v>163</v>
+        <v>272</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1615,7 +1747,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="12" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>8</v>
@@ -1626,30 +1758,29 @@
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="12" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="12" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>8</v>
@@ -1659,27 +1790,30 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="12" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>8</v>
@@ -1690,7 +1824,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="12" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>8</v>
@@ -1700,92 +1834,189 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1794,28 +2025,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L159"/>
+  <dimension ref="A1:Q183"/>
   <sheetViews>
-    <sheetView topLeftCell="E123" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K127" sqref="K127"/>
+    <sheetView topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="2"/>
@@ -1854,12 +2086,7 @@
       <c r="B3" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>160</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
@@ -1919,7 +2146,7 @@
         <v>113</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1954,7 +2181,7 @@
         <v>116</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2008,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>197</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2028,6 +2255,9 @@
       <c r="A23" s="14" t="s">
         <v>2</v>
       </c>
+      <c r="B23" s="2" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
@@ -2150,7 +2380,7 @@
         <v>64</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D38" s="24"/>
     </row>
@@ -2184,16 +2414,16 @@
         <v>49</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D42" s="23" t="s">
         <v>188</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>189</v>
       </c>
       <c r="E42" s="23" t="s">
         <v>64</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>146</v>
@@ -2207,7 +2437,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>153</v>
@@ -2232,16 +2462,16 @@
         <v>49</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="23" t="s">
         <v>188</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>189</v>
       </c>
       <c r="E46" s="23" t="s">
         <v>64</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>146</v>
@@ -2340,10 +2570,10 @@
         <v>58</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>146</v>
@@ -2352,7 +2582,7 @@
         <v>59</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -2368,10 +2598,10 @@
         <v>60</v>
       </c>
       <c r="D59" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E59" s="23" t="s">
         <v>195</v>
-      </c>
-      <c r="E59" s="23" t="s">
-        <v>196</v>
       </c>
       <c r="F59" s="2">
         <v>28139</v>
@@ -2432,7 +2662,7 @@
         <v>64</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E66" s="23" t="s">
         <v>63</v>
@@ -2477,25 +2707,25 @@
         <v>131</v>
       </c>
       <c r="D70" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E70" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="E70" s="23" t="s">
+      <c r="F70" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="H70" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="I70" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="I70" s="32" t="s">
+      <c r="J70" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -2512,22 +2742,22 @@
         <v>60</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F71" s="2">
         <v>3</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2535,7 +2765,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>1</v>
       </c>
@@ -2546,25 +2776,25 @@
         <v>131</v>
       </c>
       <c r="D74" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E74" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="E74" s="23" t="s">
+      <c r="F74" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="G74" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="H74" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="I74" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="I74" s="32" t="s">
+      <c r="J74" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -2572,7 +2802,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>130</v>
@@ -2581,22 +2811,22 @@
         <v>60</v>
       </c>
       <c r="E75" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F75" s="2">
         <v>3</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -2609,7 +2839,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C78" s="22" t="s">
         <v>71</v>
@@ -2650,10 +2880,10 @@
         <v>70130</v>
       </c>
       <c r="G79" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H79" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2672,7 +2902,7 @@
         <v>1</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C82" s="22" t="s">
         <v>71</v>
@@ -2713,10 +2943,10 @@
         <v>70130</v>
       </c>
       <c r="G83" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -2729,7 +2959,7 @@
         <v>1</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C86" s="22" t="s">
         <v>71</v>
@@ -2764,13 +2994,13 @@
         <v>132</v>
       </c>
       <c r="E87" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F87" s="2">
         <v>70130</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>127</v>
@@ -2949,7 +3179,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -2957,7 +3187,7 @@
         <v>1</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>90</v>
@@ -2980,27 +3210,27 @@
         <v>2</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D111" s="23">
         <v>100</v>
       </c>
       <c r="E111" s="35" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F111" s="33" t="s">
         <v>101</v>
       </c>
       <c r="G111" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -3008,7 +3238,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>90</v>
@@ -3031,22 +3261,22 @@
         <v>2</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D115" s="23">
         <v>100</v>
       </c>
       <c r="E115" s="35" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F115" s="33" t="s">
         <v>101</v>
       </c>
       <c r="G115" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
@@ -3097,16 +3327,16 @@
         <v>101</v>
       </c>
       <c r="D119" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="E119" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="F119" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E119" s="23" t="s">
+      <c r="G119" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="H119" s="2" t="s">
         <v>2</v>
@@ -3135,12 +3365,12 @@
         <v>2</v>
       </c>
       <c r="D123" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
@@ -3172,51 +3402,51 @@
         <v>33</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L126" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="20">
-        <v>1</v>
-      </c>
-      <c r="C127" s="2">
-        <v>10</v>
-      </c>
-      <c r="D127" s="23">
-        <v>2016</v>
-      </c>
-      <c r="E127" s="23">
-        <v>2</v>
-      </c>
-      <c r="F127" s="2">
-        <v>2</v>
-      </c>
-      <c r="G127" s="2">
-        <v>2016</v>
+      <c r="B127" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C127" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D127" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E127" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F127" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="G127" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="H127" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I127" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I127" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="J127" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>238</v>
+        <v>170</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
@@ -3224,7 +3454,7 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -3256,51 +3486,51 @@
         <v>33</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B131" s="20">
-        <v>1</v>
-      </c>
-      <c r="C131" s="2">
-        <v>10</v>
-      </c>
-      <c r="D131" s="23">
-        <v>2016</v>
-      </c>
-      <c r="E131" s="23">
-        <v>2</v>
-      </c>
-      <c r="F131" s="2">
-        <v>2</v>
-      </c>
-      <c r="G131" s="2">
-        <v>2016</v>
+      <c r="B131" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C131" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D131" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E131" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F131" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="G131" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="H131" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I131" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I131" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="J131" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L131" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
@@ -3308,7 +3538,7 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -3340,51 +3570,51 @@
         <v>33</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L134" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B135" s="20">
-        <v>1</v>
-      </c>
-      <c r="C135" s="2">
-        <v>10</v>
-      </c>
-      <c r="D135" s="23">
-        <v>2016</v>
-      </c>
-      <c r="E135" s="23">
-        <v>2</v>
-      </c>
-      <c r="F135" s="2">
-        <v>2</v>
-      </c>
-      <c r="G135" s="2">
-        <v>2016</v>
+      <c r="B135" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C135" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D135" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E135" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F135" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="G135" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="H135" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I135" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I135" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="J135" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L135" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -3392,7 +3622,7 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
@@ -3424,51 +3654,51 @@
         <v>33</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L138" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="20">
-        <v>1</v>
-      </c>
-      <c r="C139" s="2">
-        <v>10</v>
-      </c>
-      <c r="D139" s="23">
-        <v>2016</v>
-      </c>
-      <c r="E139" s="23">
-        <v>2</v>
-      </c>
-      <c r="F139" s="2">
-        <v>2</v>
-      </c>
-      <c r="G139" s="2">
-        <v>2016</v>
+      <c r="B139" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C139" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D139" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E139" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F139" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="G139" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="H139" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I139" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I139" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="J139" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K139" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L139" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
@@ -3476,7 +3706,7 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
@@ -3502,12 +3732,14 @@
         <v>109</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="J142" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>252</v>
+      </c>
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
     </row>
@@ -3515,40 +3747,43 @@
       <c r="A143" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="20">
-        <v>1</v>
-      </c>
-      <c r="C143" s="2">
-        <v>10</v>
-      </c>
-      <c r="D143" s="23">
-        <v>2016</v>
-      </c>
-      <c r="E143" s="23">
-        <v>2</v>
-      </c>
-      <c r="F143" s="2">
-        <v>2</v>
-      </c>
-      <c r="G143" s="2">
-        <v>2016</v>
+      <c r="B143" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C143" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D143" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E143" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F143" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="G143" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>169</v>
+        <v>278</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
+      </c>
+      <c r="J143" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B144" s="20"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>1</v>
       </c>
@@ -3571,76 +3806,70 @@
         <v>109</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="K146" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="L146" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="K146" s="27"/>
+      <c r="L146" s="27"/>
+      <c r="M146" s="27"/>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B147" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="C147" s="2">
-        <v>10</v>
-      </c>
-      <c r="D147" s="23">
-        <v>2016</v>
-      </c>
-      <c r="E147" s="23">
-        <v>2</v>
-      </c>
-      <c r="F147" s="2">
-        <v>2</v>
-      </c>
-      <c r="G147" s="2">
-        <v>2016</v>
+        <v>221</v>
+      </c>
+      <c r="C147" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D147" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E147" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F147" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="G147" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>173</v>
+        <v>278</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>112</v>
+        <v>280</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="K147" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="L147" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="K147" s="27"/>
+      <c r="L147" s="27"/>
+      <c r="M147" s="27"/>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B150" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C150" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>52</v>
@@ -3649,52 +3878,56 @@
         <v>33</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I150" s="27"/>
+        <v>219</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>252</v>
+      </c>
       <c r="J150" s="27"/>
       <c r="K150" s="27"/>
       <c r="L150" s="27"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B151" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="D151" t="s">
+        <v>217</v>
+      </c>
+      <c r="E151" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="D151" t="s">
-        <v>219</v>
-      </c>
-      <c r="E151" s="27" t="s">
+      <c r="F151" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G151" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F151" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G151" s="27" t="s">
+      <c r="H151" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="H151" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="I151" s="27"/>
+      <c r="I151" s="27" t="s">
+        <v>261</v>
+      </c>
       <c r="J151" s="27"/>
       <c r="K151" s="27"/>
       <c r="L151" s="27"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>1</v>
       </c>
@@ -3710,7 +3943,7 @@
       <c r="K154" s="27"/>
       <c r="L154" s="27"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>2</v>
       </c>
@@ -3724,12 +3957,12 @@
       <c r="K155" s="27"/>
       <c r="L155" s="27"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>1</v>
       </c>
@@ -3741,7 +3974,7 @@
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>2</v>
       </c>
@@ -3750,6 +3983,486 @@
       <c r="E159" s="27"/>
       <c r="G159" s="27"/>
       <c r="H159" s="27"/>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B160" s="20"/>
+      <c r="D160"/>
+      <c r="E160" s="27"/>
+      <c r="G160" s="27"/>
+      <c r="H160" s="27"/>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A161" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I162" s="27"/>
+      <c r="J162" s="27"/>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B163" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D163" t="s">
+        <v>216</v>
+      </c>
+      <c r="E163" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G163" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="H163" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="I163" s="27"/>
+      <c r="J163" s="27"/>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A165" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J166" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L166" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M166" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C167" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D167" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E167" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F167" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="G167" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I167" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J167" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="K167" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="L167" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M167" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A169" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L170" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M170" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N170" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="O170" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B171" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C171" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D171" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E171" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F171" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="G171" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I171" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J171" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="K171" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="L171" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M171" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N171" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="O171" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A173" s="19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I174" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J174" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="K174" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L174" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="O174" s="27"/>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B175" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C175" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D175" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E175" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F175" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="G175" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I175" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J175" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="K175" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L175" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="M175" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="O175" s="27"/>
+    </row>
+    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A177" s="19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H178" s="27"/>
+      <c r="I178" s="27"/>
+      <c r="J178" s="27"/>
+      <c r="K178" s="27"/>
+      <c r="L178" s="27"/>
+      <c r="M178" s="27"/>
+      <c r="N178" s="27"/>
+      <c r="O178" s="27"/>
+      <c r="P178" s="27"/>
+      <c r="Q178" s="27"/>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A179" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B179" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="C179" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="D179" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="E179" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="F179" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="G179" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="H179" s="27"/>
+      <c r="I179" s="27"/>
+      <c r="J179" s="27"/>
+      <c r="K179" s="27"/>
+      <c r="L179" s="27"/>
+      <c r="M179" s="27"/>
+      <c r="N179" s="27"/>
+      <c r="O179" s="27"/>
+      <c r="P179" s="27"/>
+      <c r="Q179" s="27"/>
+    </row>
+    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A181" s="19" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F182" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="G182" s="27"/>
+      <c r="H182" s="27"/>
+      <c r="I182" s="27"/>
+      <c r="J182" s="27"/>
+      <c r="K182" s="27"/>
+      <c r="L182" s="27"/>
+      <c r="M182" s="27"/>
+      <c r="N182" s="27"/>
+      <c r="O182" s="27"/>
+      <c r="P182" s="27"/>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A183" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B183" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="C183" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D183" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="E183" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="F183" s="42">
+        <f ca="1">NOW()</f>
+        <v>42453.529550115738</v>
+      </c>
+      <c r="G183" s="27"/>
+      <c r="H183" s="27"/>
+      <c r="I183" s="27"/>
+      <c r="J183" s="27"/>
+      <c r="K183" s="27"/>
+      <c r="L183" s="27"/>
+      <c r="M183" s="27"/>
+      <c r="N183" s="27"/>
+      <c r="O183" s="27"/>
+      <c r="P183" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3767,7 +4480,7 @@
   <dimension ref="A1:BL3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3825,7 +4538,7 @@
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3835,10 +4548,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -3907,10 +4620,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>

</xml_diff>

<commit_message>
Committing the latest changes in admin.java,adminLib.java,adminPage.java
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="768" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="768" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Browsers" sheetId="14" r:id="rId1"/>
@@ -16,14 +16,14 @@
     <sheet name="Reports" sheetId="18" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">allTests!$E$1:$E$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">allTests!$E$1:$E$82</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3400" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3416" uniqueCount="626">
   <si>
     <t>Runmode</t>
   </si>
@@ -1730,9 +1730,6 @@
     <t>SiteInReport</t>
   </si>
   <si>
-    <t>ORL</t>
-  </si>
-  <si>
     <t>Hospice</t>
   </si>
   <si>
@@ -1799,9 +1796,6 @@
     <t>Team Meeting</t>
   </si>
   <si>
-    <t>03/28/16 - 04/04/16</t>
-  </si>
-  <si>
     <t>testGenerateContactsListReport</t>
   </si>
   <si>
@@ -1889,10 +1883,25 @@
     <t>Credit Claim Balance Report</t>
   </si>
   <si>
-    <t>04/05/16</t>
-  </si>
-  <si>
     <t>ReportsUser</t>
+  </si>
+  <si>
+    <t>04/06/16</t>
+  </si>
+  <si>
+    <t>03/29/16 - 04/06/16</t>
+  </si>
+  <si>
+    <t>03/05/16 - 04/06/16</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -2322,7 +2331,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2357,7 +2366,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2781,10 +2790,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E82"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2837,7 +2847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D4" s="12" t="s">
         <v>442</v>
       </c>
@@ -2845,7 +2855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D5" s="12" t="s">
         <v>35</v>
       </c>
@@ -2853,7 +2863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D6" s="12" t="s">
         <v>38</v>
       </c>
@@ -2861,7 +2871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D7" s="12" t="s">
         <v>39</v>
       </c>
@@ -2869,7 +2879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
         <v>44</v>
       </c>
@@ -3021,7 +3031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D27" s="33" t="s">
         <v>112</v>
       </c>
@@ -3029,7 +3039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D28" s="33" t="s">
         <v>119</v>
       </c>
@@ -3133,7 +3143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D41" s="33" t="s">
         <v>422</v>
       </c>
@@ -3201,10 +3211,10 @@
         <v>360</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D49" s="33" t="s">
         <v>308</v>
       </c>
@@ -3257,7 +3267,7 @@
         <v>387</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3323,12 +3333,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" s="32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D63" s="33" t="s">
         <v>473</v>
       </c>
       <c r="E63" s="33" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3339,12 +3349,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" s="32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D65" s="33" t="s">
         <v>483</v>
       </c>
       <c r="E65" s="33" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3359,10 +3369,10 @@
       </c>
       <c r="D66" s="61"/>
       <c r="E66" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="66"/>
       <c r="B67" s="66"/>
       <c r="C67" s="66"/>
@@ -3370,7 +3380,7 @@
         <v>519</v>
       </c>
       <c r="E67" s="33" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3378,7 +3388,7 @@
         <v>11</v>
       </c>
       <c r="B68" s="87" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C68" s="87" t="s">
         <v>377</v>
@@ -3393,7 +3403,7 @@
       <c r="B69" s="88"/>
       <c r="C69" s="88"/>
       <c r="D69" s="33" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E69" s="33" t="s">
         <v>2</v>
@@ -3404,7 +3414,7 @@
       <c r="B70" s="88"/>
       <c r="C70" s="88"/>
       <c r="D70" s="33" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E70" s="33" t="s">
         <v>2</v>
@@ -3415,7 +3425,7 @@
       <c r="B71" s="88"/>
       <c r="C71" s="88"/>
       <c r="D71" s="33" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E71" s="33" t="s">
         <v>2</v>
@@ -3426,7 +3436,7 @@
       <c r="B72" s="88"/>
       <c r="C72" s="88"/>
       <c r="D72" s="33" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E72" s="33" t="s">
         <v>2</v>
@@ -3437,7 +3447,7 @@
       <c r="B73" s="88"/>
       <c r="C73" s="88"/>
       <c r="D73" s="33" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E73" s="33" t="s">
         <v>2</v>
@@ -3470,7 +3480,7 @@
       <c r="B76" s="88"/>
       <c r="C76" s="88"/>
       <c r="D76" s="33" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E76" s="33" t="s">
         <v>2</v>
@@ -3481,7 +3491,7 @@
       <c r="B77" s="88"/>
       <c r="C77" s="88"/>
       <c r="D77" s="33" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E77" s="33" t="s">
         <v>2</v>
@@ -3492,7 +3502,7 @@
       <c r="B78" s="88"/>
       <c r="C78" s="88"/>
       <c r="D78" s="33" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E78" s="33" t="s">
         <v>2</v>
@@ -3503,7 +3513,7 @@
       <c r="B79" s="88"/>
       <c r="C79" s="88"/>
       <c r="D79" s="33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E79" s="33" t="s">
         <v>2</v>
@@ -3514,7 +3524,7 @@
       <c r="B80" s="88"/>
       <c r="C80" s="88"/>
       <c r="D80" s="33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E80" s="33" t="s">
         <v>2</v>
@@ -3543,7 +3553,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E67"/>
+  <autoFilter ref="E1:E82">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3554,7 +3570,7 @@
   <dimension ref="A1:BC159"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3580,9 +3596,8 @@
     <col min="19" max="19" width="26.140625" style="32" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23.28515625" style="32" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="24.85546875" style="32" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="24.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" style="32" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8.5703125" style="32" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9.28515625" style="32" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" style="32" bestFit="1" customWidth="1"/>
@@ -5537,14 +5552,30 @@
       <c r="Q150" s="70" t="s">
         <v>269</v>
       </c>
-      <c r="R150" s="39"/>
-      <c r="S150" s="39"/>
-      <c r="T150" s="39"/>
-      <c r="U150" s="39"/>
-      <c r="V150" s="39"/>
-      <c r="W150" s="39"/>
-      <c r="X150" s="39"/>
-      <c r="Y150" s="39"/>
+      <c r="R150" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="S150" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="T150" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="U150" s="77" t="s">
+        <v>174</v>
+      </c>
+      <c r="V150" s="77" t="s">
+        <v>175</v>
+      </c>
+      <c r="W150" s="77" t="s">
+        <v>176</v>
+      </c>
+      <c r="X150" s="86" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y150" s="86" t="s">
+        <v>169</v>
+      </c>
       <c r="Z150" s="39"/>
       <c r="AA150" s="39"/>
       <c r="AB150" s="39"/>
@@ -5613,14 +5644,14 @@
       <c r="L151" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="M151" s="47" t="s">
-        <v>205</v>
-      </c>
-      <c r="N151" s="47" t="s">
-        <v>500</v>
-      </c>
-      <c r="O151" s="47" t="s">
-        <v>207</v>
+      <c r="M151" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="N151" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="O151" s="15" t="s">
+        <v>247</v>
       </c>
       <c r="P151" s="16" t="s">
         <v>268</v>
@@ -5628,14 +5659,30 @@
       <c r="Q151" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="R151" s="39"/>
-      <c r="S151" s="39"/>
-      <c r="T151" s="39"/>
-      <c r="U151" s="39"/>
-      <c r="V151" s="39"/>
-      <c r="W151" s="39"/>
-      <c r="X151" s="39"/>
-      <c r="Y151" s="39"/>
+      <c r="R151" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="S151" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="T151" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="U151" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="V151" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="W151" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="X151" s="88" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y151" s="91" t="s">
+        <v>203</v>
+      </c>
       <c r="Z151" s="39"/>
       <c r="AA151" s="39"/>
       <c r="AB151" s="39"/>
@@ -5927,8 +5974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CL72"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6:V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18196,8 +18243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18559,22 +18606,22 @@
         <v>207</v>
       </c>
       <c r="H15" s="64" t="s">
+        <v>572</v>
+      </c>
+      <c r="I15" s="64" t="s">
         <v>568</v>
-      </c>
-      <c r="I15" s="64" t="s">
-        <v>569</v>
       </c>
       <c r="J15" s="64" t="s">
         <v>563</v>
       </c>
       <c r="K15" s="64" t="s">
+        <v>569</v>
+      </c>
+      <c r="L15" s="64" t="s">
+        <v>568</v>
+      </c>
+      <c r="M15" s="64" t="s">
         <v>570</v>
-      </c>
-      <c r="L15" s="64" t="s">
-        <v>569</v>
-      </c>
-      <c r="M15" s="64" t="s">
-        <v>571</v>
       </c>
       <c r="N15" s="64"/>
       <c r="O15" s="64"/>
@@ -18616,7 +18663,7 @@
     </row>
     <row r="17" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B17" s="64"/>
       <c r="C17" s="64"/>
@@ -18699,40 +18746,40 @@
         <v>2</v>
       </c>
       <c r="B19" s="93" t="s">
-        <v>559</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>280</v>
+        <v>560</v>
+      </c>
+      <c r="C19" s="93" t="s">
+        <v>623</v>
       </c>
       <c r="D19" s="94" t="s">
         <v>207</v>
       </c>
       <c r="E19" s="94" t="s">
-        <v>560</v>
+        <v>624</v>
       </c>
       <c r="F19" s="69" t="s">
-        <v>560</v>
+        <v>625</v>
       </c>
       <c r="G19" s="69" t="s">
         <v>207</v>
       </c>
       <c r="H19" s="64" t="s">
+        <v>572</v>
+      </c>
+      <c r="I19" s="64" t="s">
+        <v>568</v>
+      </c>
+      <c r="J19" s="64" t="s">
+        <v>622</v>
+      </c>
+      <c r="K19" s="64" t="s">
+        <v>569</v>
+      </c>
+      <c r="L19" s="64" t="s">
+        <v>568</v>
+      </c>
+      <c r="M19" s="64" t="s">
         <v>573</v>
-      </c>
-      <c r="I19" s="64" t="s">
-        <v>569</v>
-      </c>
-      <c r="J19" s="64" t="s">
-        <v>563</v>
-      </c>
-      <c r="K19" s="64" t="s">
-        <v>570</v>
-      </c>
-      <c r="L19" s="64" t="s">
-        <v>569</v>
-      </c>
-      <c r="M19" s="64" t="s">
-        <v>574</v>
       </c>
       <c r="N19" s="64"/>
       <c r="O19" s="64"/>
@@ -18774,7 +18821,7 @@
     </row>
     <row r="21" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B21" s="64"/>
       <c r="C21" s="64"/>
@@ -18875,22 +18922,22 @@
         <v>207</v>
       </c>
       <c r="H23" s="64" t="s">
+        <v>572</v>
+      </c>
+      <c r="I23" s="64" t="s">
         <v>568</v>
-      </c>
-      <c r="I23" s="64" t="s">
-        <v>569</v>
       </c>
       <c r="J23" s="64" t="s">
         <v>563</v>
       </c>
       <c r="K23" s="64" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L23" s="64" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="M23" s="64" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="N23" s="64"/>
       <c r="O23" s="64"/>
@@ -18932,7 +18979,7 @@
     </row>
     <row r="25" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B25" s="64"/>
       <c r="C25" s="64"/>
@@ -19027,13 +19074,13 @@
         <v>207</v>
       </c>
       <c r="H27" s="64" t="s">
+        <v>577</v>
+      </c>
+      <c r="I27" s="64" t="s">
         <v>578</v>
       </c>
-      <c r="I27" s="64" t="s">
-        <v>579</v>
-      </c>
       <c r="J27" s="64" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K27" s="64"/>
       <c r="L27" s="64"/>
@@ -19078,7 +19125,7 @@
     </row>
     <row r="29" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="62" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B29" s="64"/>
       <c r="C29" s="64"/>
@@ -19173,13 +19220,13 @@
         <v>207</v>
       </c>
       <c r="H31" s="64" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I31" s="64" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J31" s="64" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K31" s="95"/>
       <c r="L31" s="95"/>
@@ -19224,7 +19271,7 @@
     </row>
     <row r="33" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B33" s="64"/>
       <c r="C33" s="64"/>
@@ -19255,13 +19302,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="63" t="s">
+        <v>582</v>
+      </c>
+      <c r="C34" s="63" t="s">
         <v>583</v>
       </c>
-      <c r="C34" s="63" t="s">
+      <c r="D34" s="63" t="s">
         <v>584</v>
-      </c>
-      <c r="D34" s="63" t="s">
-        <v>585</v>
       </c>
       <c r="E34" s="63" t="s">
         <v>66</v>
@@ -19273,7 +19320,7 @@
         <v>558</v>
       </c>
       <c r="H34" s="63" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I34" s="63" t="s">
         <v>567</v>
@@ -19299,28 +19346,28 @@
         <v>2</v>
       </c>
       <c r="B35" s="93" t="s">
+        <v>586</v>
+      </c>
+      <c r="C35" s="64" t="s">
         <v>587</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="D35" s="85" t="s">
         <v>588</v>
       </c>
-      <c r="D35" s="85" t="s">
-        <v>589</v>
-      </c>
       <c r="E35" s="95" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F35" s="64" t="s">
         <v>562</v>
       </c>
       <c r="G35" s="95" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H35" s="95" t="s">
-        <v>591</v>
+        <v>621</v>
       </c>
       <c r="I35" s="95" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="J35" s="95"/>
       <c r="K35" s="95"/>
@@ -19366,7 +19413,7 @@
     </row>
     <row r="37" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B37" s="64"/>
       <c r="C37" s="64"/>
@@ -19400,22 +19447,22 @@
         <v>28</v>
       </c>
       <c r="C38" s="63" t="s">
+        <v>591</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="E38" s="63" t="s">
         <v>593</v>
-      </c>
-      <c r="D38" s="63" t="s">
-        <v>594</v>
-      </c>
-      <c r="E38" s="63" t="s">
-        <v>595</v>
       </c>
       <c r="F38" s="63" t="s">
         <v>66</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H38" s="63" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="I38" s="95"/>
       <c r="J38" s="95"/>
@@ -19439,25 +19486,25 @@
         <v>2</v>
       </c>
       <c r="B39" s="93" t="s">
+        <v>596</v>
+      </c>
+      <c r="C39" s="64" t="s">
+        <v>597</v>
+      </c>
+      <c r="D39" s="85" t="s">
+        <v>572</v>
+      </c>
+      <c r="E39" s="95" t="s">
         <v>598</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="F39" s="64" t="s">
         <v>599</v>
       </c>
-      <c r="D39" s="85" t="s">
-        <v>573</v>
-      </c>
-      <c r="E39" s="95" t="s">
+      <c r="G39" s="95" t="s">
         <v>600</v>
       </c>
-      <c r="F39" s="64" t="s">
+      <c r="H39" s="95" t="s">
         <v>601</v>
-      </c>
-      <c r="G39" s="95" t="s">
-        <v>602</v>
-      </c>
-      <c r="H39" s="95" t="s">
-        <v>603</v>
       </c>
       <c r="I39" s="95"/>
       <c r="J39" s="95"/>
@@ -19504,7 +19551,7 @@
     </row>
     <row r="41" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B41" s="64"/>
       <c r="C41" s="64"/>
@@ -19562,7 +19609,7 @@
         <v>555</v>
       </c>
       <c r="K42" s="63" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L42" s="63" t="s">
         <v>557</v>
@@ -19590,7 +19637,7 @@
         <v>559</v>
       </c>
       <c r="C43" s="69" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D43" s="94" t="s">
         <v>207</v>
@@ -19605,22 +19652,22 @@
         <v>207</v>
       </c>
       <c r="H43" s="64" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I43" s="64" t="s">
+        <v>568</v>
+      </c>
+      <c r="J43" s="64" t="s">
+        <v>604</v>
+      </c>
+      <c r="K43" s="64" t="s">
+        <v>605</v>
+      </c>
+      <c r="L43" s="64" t="s">
+        <v>568</v>
+      </c>
+      <c r="M43" s="64" t="s">
         <v>569</v>
-      </c>
-      <c r="J43" s="64" t="s">
-        <v>606</v>
-      </c>
-      <c r="K43" s="64" t="s">
-        <v>607</v>
-      </c>
-      <c r="L43" s="64" t="s">
-        <v>569</v>
-      </c>
-      <c r="M43" s="64" t="s">
-        <v>570</v>
       </c>
       <c r="N43" s="64"/>
       <c r="O43" s="64"/>
@@ -19662,7 +19709,7 @@
     </row>
     <row r="45" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="62" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B45" s="64"/>
       <c r="C45" s="64"/>
@@ -19720,7 +19767,7 @@
         <v>555</v>
       </c>
       <c r="K46" s="63" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L46" s="63" t="s">
         <v>557</v>
@@ -19729,10 +19776,10 @@
         <v>567</v>
       </c>
       <c r="N46" s="63" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="O46" s="63" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="P46" s="64"/>
       <c r="Q46" s="64"/>
@@ -19752,7 +19799,7 @@
         <v>559</v>
       </c>
       <c r="C47" s="69" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D47" s="94" t="s">
         <v>207</v>
@@ -19767,28 +19814,28 @@
         <v>207</v>
       </c>
       <c r="H47" s="64" t="s">
+        <v>572</v>
+      </c>
+      <c r="I47" s="64" t="s">
         <v>568</v>
       </c>
-      <c r="I47" s="64" t="s">
+      <c r="J47" s="64" t="s">
+        <v>604</v>
+      </c>
+      <c r="K47" s="64" t="s">
+        <v>609</v>
+      </c>
+      <c r="L47" s="64" t="s">
+        <v>568</v>
+      </c>
+      <c r="M47" s="64" t="s">
         <v>569</v>
       </c>
-      <c r="J47" s="64" t="s">
-        <v>606</v>
-      </c>
-      <c r="K47" s="64" t="s">
+      <c r="N47" s="64" t="s">
+        <v>610</v>
+      </c>
+      <c r="O47" s="64" t="s">
         <v>611</v>
-      </c>
-      <c r="L47" s="64" t="s">
-        <v>569</v>
-      </c>
-      <c r="M47" s="64" t="s">
-        <v>570</v>
-      </c>
-      <c r="N47" s="64" t="s">
-        <v>612</v>
-      </c>
-      <c r="O47" s="64" t="s">
-        <v>613</v>
       </c>
       <c r="P47" s="64"/>
       <c r="Q47" s="64"/>
@@ -19828,7 +19875,7 @@
     </row>
     <row r="49" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="62" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B49" s="64"/>
       <c r="C49" s="64"/>
@@ -19877,7 +19924,7 @@
         <v>553</v>
       </c>
       <c r="H50" s="63" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I50" s="63" t="s">
         <v>66</v>
@@ -19886,10 +19933,10 @@
         <v>567</v>
       </c>
       <c r="K50" s="63" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L50" s="63" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="M50" s="63" t="s">
         <v>555</v>
@@ -19914,7 +19961,7 @@
         <v>559</v>
       </c>
       <c r="C51" s="69" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D51" s="94" t="s">
         <v>207</v>
@@ -19929,22 +19976,22 @@
         <v>207</v>
       </c>
       <c r="H51" s="95" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="I51" s="96" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J51" s="95" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K51" s="95" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L51" s="95" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="M51" s="95" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="N51" s="95"/>
       <c r="O51" s="95"/>
@@ -19986,7 +20033,7 @@
     </row>
     <row r="53" spans="1:24" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="62" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B53" s="64"/>
       <c r="C53" s="64"/>
@@ -20026,10 +20073,10 @@
         <v>567</v>
       </c>
       <c r="E54" s="63" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F54" s="95" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="G54" s="95"/>
       <c r="H54" s="95"/>
@@ -20055,19 +20102,19 @@
         <v>2</v>
       </c>
       <c r="B55" s="96" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C55" s="97" t="s">
+        <v>568</v>
+      </c>
+      <c r="D55" s="97" t="s">
         <v>569</v>
       </c>
-      <c r="D55" s="97" t="s">
-        <v>570</v>
-      </c>
       <c r="E55" s="95" t="s">
+        <v>618</v>
+      </c>
+      <c r="F55" s="98" t="s">
         <v>620</v>
-      </c>
-      <c r="F55" s="98" t="s">
-        <v>621</v>
       </c>
       <c r="G55" s="95"/>
       <c r="H55" s="95"/>

</xml_diff>